<commit_message>
Alterado campos da planilha para facil compreensão
</commit_message>
<xml_diff>
--- a/Envio.xlsx
+++ b/Envio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.pastor\Desktop\codigos site\Cursos e etc\Python\Envio de e-mails automático uzando Gmail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5C0316-CD92-4A25-B03D-6592417F8CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED88E421-8F55-4ACA-A6F5-0B544AB40354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>E-MAIL*</t>
   </si>
   <si>
-    <t>NOME+EXTENSÃO*</t>
-  </si>
-  <si>
     <t>Nome do cliente</t>
   </si>
   <si>
@@ -53,13 +50,16 @@
   </si>
   <si>
     <t>exemplo: paisagem.pdf</t>
+  </si>
+  <si>
+    <t>NOME_ANEXO+EXTENSÃO*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -142,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -152,6 +160,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -438,7 +449,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,19 +465,19 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>